<commit_message>
change NAs to 0s in common Babine data
</commit_message>
<xml_diff>
--- a/steelhead/steelhead_update_july_17_25.xlsx
+++ b/steelhead/steelhead_update_july_17_25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/steelhead/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5A8E4F-C2B4-A44D-A02D-25C7F9A9BF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38946DA4-7322-E044-A9D7-F8289145A07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="25780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,15 +160,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>84668</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
+      <xdr:colOff>101604</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>663172</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>270464</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>169147</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -191,8 +191,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="84668" y="203200"/>
-          <a:ext cx="7351837" cy="4233333"/>
+          <a:off x="101604" y="101601"/>
+          <a:ext cx="6201360" cy="3642361"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -204,15 +204,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>71967</xdr:rowOff>
+      <xdr:colOff>105835</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>646874</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>33868</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>282223</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>122893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -235,8 +235,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="88900" y="4542367"/>
-          <a:ext cx="7331307" cy="4246034"/>
+          <a:off x="105835" y="3793068"/>
+          <a:ext cx="6208888" cy="3667603"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -248,15 +248,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>84669</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>135467</xdr:rowOff>
+      <xdr:colOff>101604</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>6115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>626533</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>44706</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>270463</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>6740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -279,8 +279,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="84669" y="8890000"/>
-          <a:ext cx="7992531" cy="4752173"/>
+          <a:off x="101604" y="7532041"/>
+          <a:ext cx="6201359" cy="3763588"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A42:AH176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q76" sqref="Q76"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J61" sqref="A1:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>